<commit_message>
Klar Aks tror jag
</commit_message>
<xml_diff>
--- a/Databasteknik AKS/Volymberäkning.xlsx
+++ b/Databasteknik AKS/Volymberäkning.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,7 +598,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>264</v>
+        <v>164</v>
       </c>
       <c r="C7">
         <v>1000</v>
@@ -621,11 +621,11 @@
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>264000</v>
+        <v>164000</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>1320000</v>
+        <v>820000</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -666,11 +666,11 @@
     <row r="9" spans="1:9">
       <c r="H9">
         <f>SUM(H3:H8)</f>
-        <v>311370</v>
+        <v>211370</v>
       </c>
       <c r="I9">
         <f>SUM(I3:I8)</f>
-        <v>1522906</v>
+        <v>1022906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Klar för nu Aks Slutgiltig.
</commit_message>
<xml_diff>
--- a/Databasteknik AKS/Volymberäkning.xlsx
+++ b/Databasteknik AKS/Volymberäkning.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -496,31 +496,31 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <f>C4+500</f>
-        <v>1250</v>
+        <f>C4+1000</f>
+        <v>2000</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:G4" si="1">D4+500</f>
-        <v>1750</v>
+        <v>2500</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>2250</v>
+        <v>3000</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>2750</v>
+        <v>3500</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H8" si="2">C4*B4</f>
-        <v>10500</v>
+        <v>14000</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I8" si="3">B4*G4</f>
-        <v>38500</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -666,11 +666,11 @@
     <row r="9" spans="1:9">
       <c r="H9">
         <f>SUM(H3:H8)</f>
-        <v>211370</v>
+        <v>214870</v>
       </c>
       <c r="I9">
         <f>SUM(I3:I8)</f>
-        <v>1022906</v>
+        <v>1033406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit nu lämnar jag in skiten.
</commit_message>
<xml_diff>
--- a/Databasteknik AKS/Volymberäkning.xlsx
+++ b/Databasteknik AKS/Volymberäkning.xlsx
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,31 +531,31 @@
         <v>22</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D5">
-        <f>C5+7</f>
-        <v>17</v>
+        <f>C5+10</f>
+        <v>60</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:G5" si="4">D5+7</f>
-        <v>24</v>
+        <f t="shared" ref="E5:G5" si="4">D5+10</f>
+        <v>70</v>
       </c>
       <c r="F5">
         <f t="shared" si="4"/>
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>220</v>
+        <v>1100</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>836</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -566,31 +566,31 @@
         <v>82</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D6">
-        <f>C6+15</f>
-        <v>90</v>
+        <f>C6+10</f>
+        <v>110</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:G6" si="5">D6+15</f>
-        <v>105</v>
+        <f t="shared" ref="E6:G6" si="5">D6+20</f>
+        <v>130</v>
       </c>
       <c r="F6">
         <f t="shared" si="5"/>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="G6">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>6150</v>
+        <v>8200</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>11070</v>
+        <v>13940</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -636,41 +636,46 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="D8">
-        <f>C8+750</f>
-        <v>1500</v>
+        <f>C8+500</f>
+        <v>1000</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:G8" si="7">D8+750</f>
-        <v>2250</v>
+        <v>1750</v>
       </c>
       <c r="F8">
         <f t="shared" si="7"/>
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="G8">
         <f t="shared" si="7"/>
-        <v>3750</v>
+        <v>3250</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>22500</v>
+        <v>19500</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="H9">
         <f>SUM(H3:H8)</f>
-        <v>214870</v>
+        <v>216300</v>
       </c>
       <c r="I9">
         <f>SUM(I3:I8)</f>
-        <v>1033406</v>
+        <v>1034420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="D12">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nu e jag klar
</commit_message>
<xml_diff>
--- a/Databasteknik AKS/Volymberäkning.xlsx
+++ b/Databasteknik AKS/Volymberäkning.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -586,11 +586,11 @@
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>8200</v>
+        <v>9200</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>13940</v>
+        <v>15640</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -666,11 +666,11 @@
     <row r="9" spans="1:9">
       <c r="H9">
         <f>SUM(H3:H8)</f>
-        <v>216300</v>
+        <v>217300</v>
       </c>
       <c r="I9">
         <f>SUM(I3:I8)</f>
-        <v>1034420</v>
+        <v>1036120</v>
       </c>
     </row>
     <row r="12" spans="1:9">

</xml_diff>